<commit_message>
Increase "DACS" cost to 2000 EUR/ton
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_DACS.xlsx
+++ b/SubRES_TMPL/SubRES_DACS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8588BE-8887-46CF-8604-B8E348F096C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C161F448-AE10-4591-BAD0-46F4B0FB653B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1777,8 +1777,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1966,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>0.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">

</xml_diff>